<commit_message>
Added graphs to report
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Polytech\Теория автоматов\Labs\CellularAutomaton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Polytech\CellularAutomaton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C39B23-8203-473D-BEBC-A2E58EA2B753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78733E8-47E3-4DA6-8709-57DD15AC88AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,10 +125,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -887,7 +887,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2295,7 +2294,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="ru-RU"/>
-              <a:t>Количество живых клеток по итерациям при тороидальных </a:t>
+              <a:t>Количество живых клеток по итерациям при единичных </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" sz="2880" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -3417,9 +3416,6 @@
               <c:f>Sheet1!$G$2:$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Количество живых клеток</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>Срзнач</c:v>
                 </c:pt>
@@ -8668,151 +8664,151 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH33" sqref="AH33"/>
+    <sheetView tabSelected="1" topLeftCell="P35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="21.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="21.6" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" style="1"/>
+    <col min="1" max="1" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.6640625" style="1"/>
     <col min="9" max="9" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.7109375" style="1"/>
+    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.6640625" style="1"/>
     <col min="17" max="17" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="15.7109375" style="1"/>
+    <col min="18" max="18" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="15.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="Q1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="Q2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="Q2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" s="5">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>2</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="5">
+      <c r="I3" s="5"/>
+      <c r="J3" s="4">
         <v>1</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>2</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>3</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>4</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="5">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="4">
         <v>1</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="4">
         <v>2</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="4">
         <v>3</v>
       </c>
-      <c r="U3" s="5">
+      <c r="U3" s="4">
         <v>4</v>
       </c>
-      <c r="V3" s="5">
+      <c r="V3" s="4">
         <v>5</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A4" s="4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4" s="2">
@@ -8834,7 +8830,7 @@
         <f>AVERAGE(B4:F4)</f>
         <v>200.2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>0</v>
       </c>
       <c r="J4" s="2">
@@ -8856,7 +8852,7 @@
         <f>AVERAGE(J4:N4)</f>
         <v>200.2</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="3">
         <v>0</v>
       </c>
       <c r="R4" s="2">
@@ -8879,8 +8875,8 @@
         <v>200.2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A5" s="4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="2">
@@ -8902,7 +8898,7 @@
         <f t="shared" ref="G5:G33" si="0">AVERAGE(B5:F5)</f>
         <v>46.6</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>1</v>
       </c>
       <c r="J5" s="2">
@@ -8924,7 +8920,7 @@
         <f t="shared" ref="O5:O33" si="1">AVERAGE(J5:N5)</f>
         <v>50.6</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>1</v>
       </c>
       <c r="R5" s="2">
@@ -8947,8 +8943,8 @@
         <v>55.8</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A6" s="4">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="2">
@@ -8970,7 +8966,7 @@
         <f t="shared" si="0"/>
         <v>5.6</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>2</v>
       </c>
       <c r="J6" s="2">
@@ -8992,7 +8988,7 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>2</v>
       </c>
       <c r="R6" s="2">
@@ -9015,8 +9011,8 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A7" s="4">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
       <c r="B7" s="2">
@@ -9038,7 +9034,7 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>3</v>
       </c>
       <c r="J7" s="2">
@@ -9060,7 +9056,7 @@
         <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>3</v>
       </c>
       <c r="R7" s="2">
@@ -9083,8 +9079,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A8" s="4">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A8" s="3">
         <v>4</v>
       </c>
       <c r="B8" s="2">
@@ -9106,7 +9102,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>4</v>
       </c>
       <c r="J8" s="2">
@@ -9128,7 +9124,7 @@
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>4</v>
       </c>
       <c r="R8" s="2">
@@ -9151,8 +9147,8 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A9" s="4">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A9" s="3">
         <v>5</v>
       </c>
       <c r="B9" s="2">
@@ -9174,7 +9170,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>5</v>
       </c>
       <c r="J9" s="2">
@@ -9196,7 +9192,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>5</v>
       </c>
       <c r="R9" s="2">
@@ -9219,8 +9215,8 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A10" s="4">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A10" s="3">
         <v>6</v>
       </c>
       <c r="B10" s="2">
@@ -9242,7 +9238,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>6</v>
       </c>
       <c r="J10" s="2">
@@ -9264,7 +9260,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>6</v>
       </c>
       <c r="R10" s="2">
@@ -9287,8 +9283,8 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A11" s="4">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A11" s="3">
         <v>7</v>
       </c>
       <c r="B11" s="2">
@@ -9310,7 +9306,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>7</v>
       </c>
       <c r="J11" s="2">
@@ -9332,7 +9328,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>7</v>
       </c>
       <c r="R11" s="2">
@@ -9355,8 +9351,8 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A12" s="4">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
       <c r="B12" s="2">
@@ -9378,7 +9374,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>8</v>
       </c>
       <c r="J12" s="2">
@@ -9400,7 +9396,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>8</v>
       </c>
       <c r="R12" s="2">
@@ -9423,8 +9419,8 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A13" s="4">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A13" s="3">
         <v>9</v>
       </c>
       <c r="B13" s="2">
@@ -9446,7 +9442,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>9</v>
       </c>
       <c r="J13" s="2">
@@ -9468,7 +9464,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>9</v>
       </c>
       <c r="R13" s="2">
@@ -9491,8 +9487,8 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A14" s="4">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A14" s="3">
         <v>10</v>
       </c>
       <c r="B14" s="2">
@@ -9514,7 +9510,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>10</v>
       </c>
       <c r="J14" s="2">
@@ -9536,7 +9532,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>10</v>
       </c>
       <c r="R14" s="2">
@@ -9559,8 +9555,8 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A15" s="4">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A15" s="3">
         <v>11</v>
       </c>
       <c r="B15" s="2">
@@ -9582,7 +9578,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>11</v>
       </c>
       <c r="J15" s="2">
@@ -9604,7 +9600,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>11</v>
       </c>
       <c r="R15" s="2">
@@ -9627,8 +9623,8 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A16" s="4">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A16" s="3">
         <v>12</v>
       </c>
       <c r="B16" s="2">
@@ -9650,7 +9646,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>12</v>
       </c>
       <c r="J16" s="2">
@@ -9672,7 +9668,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>12</v>
       </c>
       <c r="R16" s="2">
@@ -9695,8 +9691,8 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A17" s="4">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A17" s="3">
         <v>13</v>
       </c>
       <c r="B17" s="2">
@@ -9718,7 +9714,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>13</v>
       </c>
       <c r="J17" s="2">
@@ -9740,7 +9736,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>13</v>
       </c>
       <c r="R17" s="2">
@@ -9763,8 +9759,8 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A18" s="4">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A18" s="3">
         <v>14</v>
       </c>
       <c r="B18" s="2">
@@ -9786,7 +9782,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>14</v>
       </c>
       <c r="J18" s="2">
@@ -9808,7 +9804,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="Q18" s="3">
         <v>14</v>
       </c>
       <c r="R18" s="2">
@@ -9831,8 +9827,8 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A19" s="4">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A19" s="3">
         <v>15</v>
       </c>
       <c r="B19" s="2">
@@ -9854,7 +9850,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>15</v>
       </c>
       <c r="J19" s="2">
@@ -9876,7 +9872,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="Q19" s="3">
         <v>15</v>
       </c>
       <c r="R19" s="2">
@@ -9899,8 +9895,8 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A20" s="4">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A20" s="3">
         <v>16</v>
       </c>
       <c r="B20" s="2">
@@ -9922,7 +9918,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>16</v>
       </c>
       <c r="J20" s="2">
@@ -9944,7 +9940,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="Q20" s="3">
         <v>16</v>
       </c>
       <c r="R20" s="2">
@@ -9967,8 +9963,8 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A21" s="4">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A21" s="3">
         <v>17</v>
       </c>
       <c r="B21" s="2">
@@ -9990,7 +9986,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="3">
         <v>17</v>
       </c>
       <c r="J21" s="2">
@@ -10012,7 +10008,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="Q21" s="3">
         <v>17</v>
       </c>
       <c r="R21" s="2">
@@ -10035,8 +10031,8 @@
         <v>72.2</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A22" s="4">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A22" s="3">
         <v>18</v>
       </c>
       <c r="B22" s="2">
@@ -10058,7 +10054,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>18</v>
       </c>
       <c r="J22" s="2">
@@ -10080,7 +10076,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <v>18</v>
       </c>
       <c r="R22" s="2">
@@ -10103,8 +10099,8 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A23" s="4">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A23" s="3">
         <v>19</v>
       </c>
       <c r="B23" s="2">
@@ -10126,7 +10122,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>19</v>
       </c>
       <c r="J23" s="2">
@@ -10148,7 +10144,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <v>19</v>
       </c>
       <c r="R23" s="2">
@@ -10171,8 +10167,8 @@
         <v>88.8</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A24" s="4">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A24" s="3">
         <v>20</v>
       </c>
       <c r="B24" s="2">
@@ -10194,7 +10190,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="3">
         <v>20</v>
       </c>
       <c r="J24" s="2">
@@ -10216,7 +10212,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <v>20</v>
       </c>
       <c r="R24" s="2">
@@ -10239,8 +10235,8 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A25" s="4">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A25" s="3">
         <v>21</v>
       </c>
       <c r="B25" s="2">
@@ -10262,7 +10258,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="3">
         <v>21</v>
       </c>
       <c r="J25" s="2">
@@ -10284,7 +10280,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <v>21</v>
       </c>
       <c r="R25" s="2">
@@ -10307,8 +10303,8 @@
         <v>104.8</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A26" s="4">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A26" s="3">
         <v>22</v>
       </c>
       <c r="B26" s="2">
@@ -10330,7 +10326,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
         <v>22</v>
       </c>
       <c r="J26" s="2">
@@ -10352,7 +10348,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <v>22</v>
       </c>
       <c r="R26" s="2">
@@ -10375,8 +10371,8 @@
         <v>111.4</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A27" s="4">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A27" s="3">
         <v>23</v>
       </c>
       <c r="B27" s="2">
@@ -10398,7 +10394,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="3">
         <v>23</v>
       </c>
       <c r="J27" s="2">
@@ -10420,7 +10416,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <v>23</v>
       </c>
       <c r="R27" s="2">
@@ -10443,8 +10439,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A28" s="4">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A28" s="3">
         <v>24</v>
       </c>
       <c r="B28" s="2">
@@ -10466,7 +10462,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
         <v>24</v>
       </c>
       <c r="J28" s="2">
@@ -10488,7 +10484,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <v>24</v>
       </c>
       <c r="R28" s="2">
@@ -10511,8 +10507,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A29" s="4">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A29" s="3">
         <v>25</v>
       </c>
       <c r="B29" s="2">
@@ -10534,7 +10530,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="3">
         <v>25</v>
       </c>
       <c r="J29" s="2">
@@ -10556,7 +10552,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <v>25</v>
       </c>
       <c r="R29" s="2">
@@ -10579,8 +10575,8 @@
         <v>123.6</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A30" s="4">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A30" s="3">
         <v>26</v>
       </c>
       <c r="B30" s="2">
@@ -10602,7 +10598,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="3">
         <v>26</v>
       </c>
       <c r="J30" s="2">
@@ -10624,7 +10620,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <v>26</v>
       </c>
       <c r="R30" s="2">
@@ -10647,8 +10643,8 @@
         <v>124.6</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A31" s="4">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A31" s="3">
         <v>27</v>
       </c>
       <c r="B31" s="2">
@@ -10670,7 +10666,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="3">
         <v>27</v>
       </c>
       <c r="J31" s="2">
@@ -10692,7 +10688,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31" s="3">
         <v>27</v>
       </c>
       <c r="R31" s="2">
@@ -10715,8 +10711,8 @@
         <v>124.2</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A32" s="4">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A32" s="3">
         <v>28</v>
       </c>
       <c r="B32" s="2">
@@ -10738,7 +10734,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
         <v>28</v>
       </c>
       <c r="J32" s="2">
@@ -10760,7 +10756,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32" s="3">
         <v>28</v>
       </c>
       <c r="R32" s="2">
@@ -10783,8 +10779,8 @@
         <v>122.2</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.4">
-      <c r="A33" s="4">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.5">
+      <c r="A33" s="3">
         <v>30</v>
       </c>
       <c r="B33" s="2">
@@ -10806,7 +10802,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="3">
         <v>30</v>
       </c>
       <c r="J33" s="2">
@@ -10828,7 +10824,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q33" s="3">
         <v>30</v>
       </c>
       <c r="R33" s="2">

</xml_diff>